<commit_message>
fix: corrigido bug da verificação da coluna relatório gerado
</commit_message>
<xml_diff>
--- a/src/planilha_fiscalizacao.xlsx
+++ b/src/planilha_fiscalizacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz.defreitas\projects\gerador-de-relatorios\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669D8135-42CB-420F-9D8E-091FDE078171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC56D43-5B1D-4254-B56A-342AFF16E450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,12 +150,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -504,7 +498,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,9 +719,11 @@
       <c r="L5" t="s">
         <v>23</v>
       </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Relatorio Energia e Gas
</commit_message>
<xml_diff>
--- a/src/planilha_fiscalizacao.xlsx
+++ b/src/planilha_fiscalizacao.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2745" yWindow="1725" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Fiscalizações" sheetId="1" state="visible" r:id="rId1"/>
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,517 +610,7 @@
         </is>
       </c>
       <c r="K2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="n">
-        <v>45817</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10:00:07</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/15</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2032</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="n">
-        <v>45818</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>10:00:08</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/16</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2033</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="n">
-        <v>45819</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>10:00:09</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/17</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2034</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="n">
-        <v>45820</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>10:00:10</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/18</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2035</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="n">
-        <v>45821</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>10:00:11</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/19</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2036</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="n">
-        <v>45822</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>10:00:12</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/20</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2037</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="n">
-        <v>45823</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>10:00:13</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/21</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2038</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="n">
-        <v>45824</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>10:00:14</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/22</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2039</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="n">
-        <v>45825</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>10:00:15</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Joao Recife Pessoas</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/23</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2040</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="n">
-        <v>45826</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>10:00:16</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Recife</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Terminal Rodoviário do Recife - TIP</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Alcides Vieira, Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Maria Ângela Albuquerque de Freitas</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Nº 1.041.080/24</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>26/04/2025 a 01/05/2041</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Alcides Vieira;Enildo Manoel</t>
-        </is>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>